<commit_message>
Lysosomes protocol initial setup
</commit_message>
<xml_diff>
--- a/analysis/data/optobiology.xlsx
+++ b/analysis/data/optobiology.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/janpiotraschke/git_repos/fachkurs_optobiology/analysis/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3514E85D-8C22-484C-9AD7-D909156B24C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A676DCB5-1793-014E-A359-CA96B9AB0B41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15800" xr2:uid="{0747FCF5-9BB9-A240-971F-88470ED95DB6}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15800" activeTab="2" xr2:uid="{0747FCF5-9BB9-A240-971F-88470ED95DB6}"/>
   </bookViews>
   <sheets>
     <sheet name="1a-MT detyrosination" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="148">
   <si>
     <t>-</t>
   </si>
@@ -569,11 +569,87 @@
   <si>
     <t xml:space="preserve">Wellanzahl: </t>
   </si>
+  <si>
+    <t xml:space="preserve">Student 1 </t>
+  </si>
+  <si>
+    <t>Student 2</t>
+  </si>
+  <si>
+    <t>DMEM</t>
+  </si>
+  <si>
+    <t>Fugene</t>
+  </si>
+  <si>
+    <t>lamp1 DNA</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">uL </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>per Well</t>
+    </r>
+  </si>
+  <si>
+    <t>delute the DNA with the 10x H2O volume</t>
+  </si>
+  <si>
+    <t>first add the DMEM</t>
+  </si>
+  <si>
+    <t>then add the fugene and mix carefully</t>
+  </si>
+  <si>
+    <t>incubate for 5min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">add the DNA and mix </t>
+  </si>
+  <si>
+    <t>Preparation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">incubate for 15-20min at room temperature </t>
+  </si>
+  <si>
+    <t xml:space="preserve">repeat the transfection protocoll for the other well </t>
+  </si>
+  <si>
+    <t>preheat 15ml growing Medium in the water bath to 37°C</t>
+  </si>
+  <si>
+    <t>change the medium of the COS-7 cells to fresh medium</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transfection Protocol </t>
+  </si>
+  <si>
+    <t>Prepare the transfection mix in an Epi:</t>
+  </si>
+  <si>
+    <t>incubate</t>
+  </si>
+  <si>
+    <t>add 200uL of each transfection mix dropwise to a well</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="169" formatCode="0.0"/>
+  </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -615,7 +691,7 @@
       <name val="Calibri (Textkörper)"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -658,8 +734,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="17">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -861,11 +943,41 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -988,6 +1100,11 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1312,8 +1429,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E32C55F2-64D1-5747-8AFC-58CEA49DB674}">
   <dimension ref="A1:R126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="J112" sqref="J112"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="Q11" sqref="I5:Q11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2481,12 +2598,306 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B418F536-D2A8-4F42-BEB3-EBF867EDFB00}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H51"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="1.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="1"/>
+      <c r="B1" s="2">
+        <v>44739</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="1"/>
+    </row>
+    <row r="3" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="7"/>
+      <c r="B3" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="1"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="1"/>
+      <c r="B5" s="38" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="1"/>
+      <c r="B6" s="38" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="1"/>
+      <c r="B7" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="1"/>
+      <c r="B8" s="38" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="1"/>
+      <c r="B9" s="38" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="1"/>
+      <c r="B10" s="38" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="1"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="1"/>
+    </row>
+    <row r="13" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="7"/>
+      <c r="B13" s="8" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="1"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="1"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="1"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="1"/>
+      <c r="C19" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="1"/>
+      <c r="B20" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20" s="62">
+        <f>2*200</f>
+        <v>400</v>
+      </c>
+      <c r="D20" s="62">
+        <v>9.6</v>
+      </c>
+      <c r="E20" s="62">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" s="1"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" s="1"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" s="1"/>
+      <c r="B23" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" s="1"/>
+    </row>
+    <row r="25" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C25" s="1"/>
+      <c r="D25" t="s">
+        <v>46</v>
+      </c>
+      <c r="E25" t="s">
+        <v>128</v>
+      </c>
+      <c r="F25" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C26" s="1"/>
+      <c r="D26" s="60"/>
+      <c r="E26" s="59"/>
+      <c r="F26" s="58"/>
+    </row>
+    <row r="27" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C27" s="1"/>
+      <c r="D27" s="61"/>
+      <c r="E27" s="59"/>
+      <c r="F27" s="58"/>
+    </row>
+    <row r="29" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="7"/>
+      <c r="B30" s="8" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B32" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B33" s="3"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F34" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="G34" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="H34" s="9" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E35" t="s">
+        <v>133</v>
+      </c>
+      <c r="F35" s="62">
+        <v>200</v>
+      </c>
+      <c r="G35" s="62">
+        <v>4.8</v>
+      </c>
+      <c r="H35" s="62">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>0</v>
+      </c>
+      <c r="D37" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>0</v>
+      </c>
+      <c r="D38" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>0</v>
+      </c>
+      <c r="D39" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>0</v>
+      </c>
+      <c r="D40" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>0</v>
+      </c>
+      <c r="D42" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>0</v>
+      </c>
+      <c r="D44" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>0</v>
+      </c>
+      <c r="B47" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>0</v>
+      </c>
+      <c r="B49" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>0</v>
+      </c>
+      <c r="B51" t="s">
+        <v>146</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>